<commit_message>
created findDestination() and rateSection()
</commit_message>
<xml_diff>
--- a/docs/Spielfeld.xlsx
+++ b/docs/Spielfeld.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Studium\Semester2\AI\Projekt 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pascal\Documents\GitHub\AI-Zaip\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -92,7 +96,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -180,11 +184,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -211,6 +256,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -493,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AG33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AL18" sqref="AL18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AR25" sqref="AR25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -514,7 +563,7 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="J2" s="6"/>
       <c r="K2" s="8"/>
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
@@ -530,7 +579,7 @@
       <c r="W2" s="9"/>
       <c r="X2" s="7"/>
       <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
+      <c r="Z2" s="6"/>
       <c r="AA2" s="7"/>
       <c r="AB2" s="7"/>
       <c r="AC2" s="7"/>
@@ -550,23 +599,23 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="2"/>
+      <c r="J3" s="26"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
+      <c r="N3" s="11"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
+      <c r="R3" s="11"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
+      <c r="V3" s="11"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
-      <c r="Z3" s="1"/>
+      <c r="Z3" s="11"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
@@ -586,23 +635,23 @@
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="J4" s="26"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
+      <c r="N4" s="11"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
+      <c r="R4" s="11"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
+      <c r="V4" s="11"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
+      <c r="Z4" s="26"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
@@ -622,23 +671,23 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="J5" s="11"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+      <c r="N5" s="11"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
+      <c r="R5" s="11"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
+      <c r="V5" s="11"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
+      <c r="Z5" s="11"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="3"/>
@@ -657,25 +706,25 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="23"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="7"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="1"/>
@@ -694,23 +743,23 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="J7" s="11"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+      <c r="N7" s="11"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
+      <c r="R7" s="11"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
+      <c r="V7" s="11"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
+      <c r="Z7" s="11"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="2"/>
@@ -730,23 +779,23 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="J8" s="11"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+      <c r="N8" s="11"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
+      <c r="R8" s="11"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
+      <c r="V8" s="11"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
+      <c r="Z8" s="11"/>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
@@ -762,31 +811,31 @@
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="14"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="J9" s="11"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
+      <c r="N9" s="11"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
+      <c r="R9" s="11"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
+      <c r="V9" s="11"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
+      <c r="Z9" s="11"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
-      <c r="AD9" s="1"/>
+      <c r="AD9" s="11"/>
       <c r="AE9" s="2"/>
       <c r="AF9" s="1"/>
       <c r="AG9" s="12"/>
@@ -797,32 +846,32 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
-      <c r="AD10" s="1"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="6"/>
       <c r="AE10" s="2"/>
       <c r="AF10" s="2"/>
       <c r="AG10" s="12"/>
@@ -834,31 +883,31 @@
       <c r="C11" s="2"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="11"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="J11" s="11"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
+      <c r="N11" s="11"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
+      <c r="R11" s="11"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
+      <c r="V11" s="11"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
+      <c r="Z11" s="11"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
-      <c r="AD11" s="1"/>
+      <c r="AD11" s="11"/>
       <c r="AE11" s="1"/>
       <c r="AF11" s="2"/>
       <c r="AG11" s="12"/>
@@ -870,31 +919,31 @@
       <c r="C12" s="2"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="11"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="J12" s="11"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="N12" s="11"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
+      <c r="R12" s="11"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
+      <c r="V12" s="11"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
+      <c r="Z12" s="11"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
-      <c r="AD12" s="1"/>
+      <c r="AD12" s="11"/>
       <c r="AE12" s="1"/>
       <c r="AF12" s="2"/>
       <c r="AG12" s="13"/>
@@ -903,36 +952,36 @@
       <c r="B13" s="21">
         <v>20</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1"/>
-      <c r="AD13" s="1"/>
-      <c r="AE13" s="1"/>
-      <c r="AF13" s="1"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="14"/>
+      <c r="AA13" s="4"/>
+      <c r="AB13" s="4"/>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="14"/>
+      <c r="AE13" s="4"/>
+      <c r="AF13" s="4"/>
       <c r="AG13" s="13"/>
     </row>
     <row r="14" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -942,31 +991,31 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="F14" s="11"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="J14" s="11"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
+      <c r="N14" s="11"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
+      <c r="P14" s="6"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
+      <c r="R14" s="11"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
+      <c r="V14" s="11"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
+      <c r="Z14" s="11"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
-      <c r="AD14" s="1"/>
+      <c r="AD14" s="11"/>
       <c r="AE14" s="1"/>
       <c r="AF14" s="1"/>
       <c r="AG14" s="13"/>
@@ -978,31 +1027,31 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="J15" s="11"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
+      <c r="N15" s="11"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
+      <c r="P15" s="11"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
+      <c r="R15" s="11"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
+      <c r="V15" s="11"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
+      <c r="Z15" s="11"/>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
-      <c r="AD15" s="1"/>
+      <c r="AD15" s="11"/>
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
       <c r="AG15" s="13"/>
@@ -1011,36 +1060,36 @@
       <c r="B16" s="21">
         <v>17</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
-      <c r="AD16" s="1"/>
-      <c r="AE16" s="1"/>
-      <c r="AF16" s="1"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="7"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="6"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="7"/>
       <c r="AG16" s="13"/>
     </row>
     <row r="17" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1050,31 +1099,31 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="F17" s="14"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="J17" s="14"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
+      <c r="N17" s="14"/>
       <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="11"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
+      <c r="V17" s="14"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
+      <c r="Z17" s="14"/>
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
-      <c r="AD17" s="1"/>
+      <c r="AD17" s="14"/>
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
       <c r="AG17" s="13"/>
@@ -1083,36 +1132,36 @@
       <c r="B18" s="21">
         <v>15</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
-      <c r="AC18" s="1"/>
-      <c r="AD18" s="1"/>
-      <c r="AE18" s="1"/>
-      <c r="AF18" s="1"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="7"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="7"/>
+      <c r="AE18" s="7"/>
+      <c r="AF18" s="7"/>
       <c r="AG18" s="13"/>
     </row>
     <row r="19" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1134,7 +1183,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
+      <c r="R19" s="11"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
@@ -1170,7 +1219,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
+      <c r="R20" s="11"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
@@ -1206,7 +1255,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
+      <c r="R21" s="11"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
@@ -1242,7 +1291,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
+      <c r="R22" s="11"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
@@ -1278,7 +1327,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
+      <c r="R23" s="11"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
@@ -1314,7 +1363,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
+      <c r="R24" s="11"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
@@ -1350,7 +1399,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
+      <c r="R25" s="11"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
@@ -1386,7 +1435,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
+      <c r="R26" s="11"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
@@ -1422,7 +1471,7 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
+      <c r="R27" s="11"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
@@ -1458,7 +1507,7 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
+      <c r="R28" s="11"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
@@ -1494,7 +1543,7 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
+      <c r="R29" s="11"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
@@ -1530,7 +1579,7 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
+      <c r="R30" s="11"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
@@ -1566,7 +1615,7 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
+      <c r="R31" s="11"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
@@ -1602,7 +1651,7 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
+      <c r="R32" s="11"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
@@ -1727,7 +1776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AG33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
hotfix und neues zeug
Wegpunkte werden richtig abgelaufen
Stein 0 bleibt kurz stehen
</commit_message>
<xml_diff>
--- a/docs/Spielfeld.xlsx
+++ b/docs/Spielfeld.xlsx
@@ -244,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -283,6 +283,8 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -563,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AG33"/>
+  <dimension ref="B2:AO33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AO27" sqref="AO27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="Z23" sqref="Z23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1117,7 @@
       <c r="AF16" s="7"/>
       <c r="AG16" s="13"/>
     </row>
-    <row r="17" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="21">
         <v>16</v>
       </c>
@@ -1151,7 +1153,7 @@
       <c r="AF17" s="1"/>
       <c r="AG17" s="13"/>
     </row>
-    <row r="18" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="21">
         <v>15</v>
       </c>
@@ -1187,7 +1189,7 @@
       <c r="AF18" s="7"/>
       <c r="AG18" s="13"/>
     </row>
-    <row r="19" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="21">
         <v>14</v>
       </c>
@@ -1223,7 +1225,7 @@
       <c r="AF19" s="1"/>
       <c r="AG19" s="13"/>
     </row>
-    <row r="20" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="21">
         <v>13</v>
       </c>
@@ -1259,7 +1261,7 @@
       <c r="AF20" s="1"/>
       <c r="AG20" s="13"/>
     </row>
-    <row r="21" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="21">
         <v>12</v>
       </c>
@@ -1282,7 +1284,7 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
+      <c r="V21" s="28"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
@@ -1295,7 +1297,7 @@
       <c r="AF21" s="1"/>
       <c r="AG21" s="13"/>
     </row>
-    <row r="22" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="21">
         <v>11</v>
       </c>
@@ -1331,7 +1333,7 @@
       <c r="AF22" s="1"/>
       <c r="AG22" s="13"/>
     </row>
-    <row r="23" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="21">
         <v>10</v>
       </c>
@@ -1358,7 +1360,7 @@
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
-      <c r="Z23" s="1"/>
+      <c r="Z23" s="28"/>
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
@@ -1367,7 +1369,7 @@
       <c r="AF23" s="2"/>
       <c r="AG23" s="13"/>
     </row>
-    <row r="24" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="11">
         <v>9</v>
       </c>
@@ -1403,7 +1405,7 @@
       <c r="AF24" s="2"/>
       <c r="AG24" s="12"/>
     </row>
-    <row r="25" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="11">
         <v>8</v>
       </c>
@@ -1439,7 +1441,7 @@
       <c r="AF25" s="2"/>
       <c r="AG25" s="12"/>
     </row>
-    <row r="26" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="11">
         <v>7</v>
       </c>
@@ -1462,8 +1464,8 @@
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
+      <c r="V26" s="28"/>
+      <c r="W26" s="28"/>
       <c r="X26" s="1"/>
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
@@ -1475,7 +1477,7 @@
       <c r="AF26" s="1"/>
       <c r="AG26" s="12"/>
     </row>
-    <row r="27" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="11">
         <v>6</v>
       </c>
@@ -1498,8 +1500,8 @@
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
+      <c r="V27" s="28"/>
+      <c r="W27" s="28"/>
       <c r="X27" s="1"/>
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
@@ -1510,8 +1512,9 @@
       <c r="AE27" s="2"/>
       <c r="AF27" s="1"/>
       <c r="AG27" s="12"/>
-    </row>
-    <row r="28" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AO27" s="38"/>
+    </row>
+    <row r="28" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="11">
         <v>5</v>
       </c>
@@ -1547,7 +1550,7 @@
       <c r="AF28" s="1"/>
       <c r="AG28" s="12"/>
     </row>
-    <row r="29" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="11">
         <v>4</v>
       </c>
@@ -1566,7 +1569,7 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
-      <c r="R29" s="11"/>
+      <c r="R29" s="39"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
@@ -1583,7 +1586,7 @@
       <c r="AF29" s="1"/>
       <c r="AG29" s="12"/>
     </row>
-    <row r="30" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="11">
         <v>3</v>
       </c>
@@ -1601,11 +1604,11 @@
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="11"/>
+      <c r="Q30" s="28"/>
+      <c r="R30" s="39"/>
       <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-      <c r="U30" s="1"/>
+      <c r="T30" s="28"/>
+      <c r="U30" s="28"/>
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
@@ -1619,7 +1622,7 @@
       <c r="AF30" s="1"/>
       <c r="AG30" s="12"/>
     </row>
-    <row r="31" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="11">
         <v>2</v>
       </c>
@@ -1655,7 +1658,7 @@
       <c r="AF31" s="1"/>
       <c r="AG31" s="12"/>
     </row>
-    <row r="32" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="11">
         <v>1</v>
       </c>
@@ -1673,9 +1676,9 @@
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
+      <c r="Q32" s="28"/>
       <c r="R32" s="11"/>
-      <c r="S32" s="1"/>
+      <c r="S32" s="28"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>

</xml_diff>